<commit_message>
Fix datatable test1 id
</commit_message>
<xml_diff>
--- a/Samples~/DataTable/Excel/Test1.xlsx
+++ b/Samples~/DataTable/Excel/Test1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Project\GameFramework\RawTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Project\GameFramework\Assets\Samples\DataTable\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E72285-3326-4C11-8C4C-2C799F737975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76869E4B-5C8F-45F9-82B4-33C16B1F2393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="50">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,58 +35,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Id1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Id2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>e</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>i</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>j</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>float</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -274,7 +222,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Id3</t>
+    <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -600,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C14"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -613,260 +561,236 @@
     <col min="4" max="4" width="6.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" t="s">
-        <v>24</v>
-      </c>
       <c r="I1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="L1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="M1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="N1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="O1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="P1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="Q1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="R1" t="s">
-        <v>57</v>
-      </c>
-      <c r="S1" t="s">
-        <v>58</v>
-      </c>
-      <c r="T1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="O2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="P2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="Q2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="R2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" t="s">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>47</v>
       </c>
-      <c r="P3" t="s">
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" t="s">
         <v>48</v>
       </c>
-      <c r="Q3" t="s">
-        <v>49</v>
-      </c>
-      <c r="R3" t="s">
-        <v>50</v>
-      </c>
-      <c r="S3" t="s">
-        <v>51</v>
-      </c>
-      <c r="T3" t="s">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" t="s">
-        <v>60</v>
-      </c>
-      <c r="M4" t="s">
-        <v>60</v>
-      </c>
-      <c r="N4" t="s">
-        <v>60</v>
-      </c>
-      <c r="O4" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>60</v>
-      </c>
-      <c r="R4" t="s">
-        <v>60</v>
-      </c>
-      <c r="S4" t="s">
-        <v>60</v>
-      </c>
-      <c r="T4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -875,60 +799,54 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="I5">
         <v>1.01</v>
       </c>
-      <c r="J5">
-        <v>1.01</v>
-      </c>
-      <c r="K5">
-        <v>1.01</v>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="M5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="N5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="O5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="P5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="Q5" t="s">
-        <v>40</v>
-      </c>
-      <c r="R5" t="s">
-        <v>40</v>
-      </c>
-      <c r="S5" t="s">
-        <v>40</v>
-      </c>
-      <c r="T5">
+        <v>27</v>
+      </c>
+      <c r="R5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
+      <c r="B6">
+        <v>1</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -937,60 +855,54 @@
         <v>2</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>2.02</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>2.02</v>
       </c>
       <c r="I6">
         <v>2.02</v>
       </c>
-      <c r="J6">
-        <v>2.02</v>
-      </c>
-      <c r="K6">
-        <v>2.02</v>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
       </c>
       <c r="L6" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="M6" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="N6" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="O6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="P6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="Q6" t="s">
-        <v>41</v>
-      </c>
-      <c r="R6" t="s">
-        <v>41</v>
-      </c>
-      <c r="S6" t="s">
-        <v>41</v>
-      </c>
-      <c r="T6">
+        <v>28</v>
+      </c>
+      <c r="R6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
+      <c r="B7">
+        <v>0</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -999,60 +911,54 @@
         <v>3</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>3.03</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>3.03</v>
       </c>
       <c r="I7">
         <v>3.03</v>
       </c>
-      <c r="J7">
-        <v>3.03</v>
-      </c>
-      <c r="K7">
-        <v>3.03</v>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="M7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="N7" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="O7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="P7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="Q7" t="s">
-        <v>42</v>
-      </c>
-      <c r="R7" t="s">
-        <v>42</v>
-      </c>
-      <c r="S7" t="s">
-        <v>42</v>
-      </c>
-      <c r="T7">
+        <v>29</v>
+      </c>
+      <c r="R7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
+      <c r="B8">
+        <v>1</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -1061,60 +967,54 @@
         <v>4</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>4.04</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>4.04</v>
       </c>
       <c r="I8">
         <v>4.04</v>
       </c>
-      <c r="J8">
-        <v>4.04</v>
-      </c>
-      <c r="K8">
-        <v>4.04</v>
+      <c r="J8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
       </c>
       <c r="L8" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="M8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="N8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="O8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="P8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="Q8" t="s">
-        <v>43</v>
-      </c>
-      <c r="R8" t="s">
-        <v>43</v>
-      </c>
-      <c r="S8" t="s">
-        <v>43</v>
-      </c>
-      <c r="T8">
+        <v>30</v>
+      </c>
+      <c r="R8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
+      <c r="B9">
+        <v>0</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -1123,60 +1023,54 @@
         <v>5</v>
       </c>
       <c r="G9">
-        <v>5</v>
+        <v>5.05</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>5.05</v>
       </c>
       <c r="I9">
         <v>5.05</v>
       </c>
-      <c r="J9">
-        <v>5.05</v>
-      </c>
-      <c r="K9">
-        <v>5.05</v>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M9" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="N9" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="O9" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="P9" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="Q9" t="s">
-        <v>44</v>
-      </c>
-      <c r="R9" t="s">
-        <v>44</v>
-      </c>
-      <c r="S9" t="s">
-        <v>44</v>
-      </c>
-      <c r="T9">
+        <v>31</v>
+      </c>
+      <c r="R9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
+      <c r="B10">
+        <v>1</v>
       </c>
       <c r="C10">
         <v>6</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E10">
         <v>6</v>
@@ -1185,22 +1079,22 @@
         <v>6</v>
       </c>
       <c r="G10">
-        <v>6</v>
+        <v>6.06</v>
       </c>
       <c r="H10">
-        <v>6</v>
+        <v>6.06</v>
       </c>
       <c r="I10">
         <v>6.06</v>
       </c>
       <c r="J10">
-        <v>6.06</v>
+        <v>1</v>
       </c>
       <c r="K10">
-        <v>6.06</v>
+        <v>6</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M10">
         <v>6</v>
@@ -1209,36 +1103,30 @@
         <v>6</v>
       </c>
       <c r="O10">
-        <v>6</v>
+        <v>6.06</v>
       </c>
       <c r="P10">
-        <v>6</v>
+        <v>6.06</v>
       </c>
       <c r="Q10">
         <v>6.06</v>
       </c>
       <c r="R10">
-        <v>6.06</v>
-      </c>
-      <c r="S10">
-        <v>6.06</v>
-      </c>
-      <c r="T10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
+      <c r="B11">
+        <v>0</v>
       </c>
       <c r="C11">
         <v>7</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E11">
         <v>7</v>
@@ -1247,22 +1135,22 @@
         <v>7</v>
       </c>
       <c r="G11">
-        <v>7</v>
+        <v>7.07</v>
       </c>
       <c r="H11">
-        <v>7</v>
+        <v>7.07</v>
       </c>
       <c r="I11">
         <v>7.07</v>
       </c>
       <c r="J11">
-        <v>7.07</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>7.07</v>
+        <v>7</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M11">
         <v>7</v>
@@ -1271,36 +1159,30 @@
         <v>7</v>
       </c>
       <c r="O11">
-        <v>7</v>
+        <v>7.07</v>
       </c>
       <c r="P11">
-        <v>7</v>
+        <v>7.07</v>
       </c>
       <c r="Q11">
         <v>7.07</v>
       </c>
       <c r="R11">
-        <v>7.07</v>
-      </c>
-      <c r="S11">
-        <v>7.07</v>
-      </c>
-      <c r="T11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
+      <c r="B12">
+        <v>1</v>
       </c>
       <c r="C12">
         <v>8</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E12">
         <v>8</v>
@@ -1309,22 +1191,22 @@
         <v>8</v>
       </c>
       <c r="G12">
-        <v>8</v>
+        <v>8.08</v>
       </c>
       <c r="H12">
-        <v>8</v>
+        <v>8.08</v>
       </c>
       <c r="I12">
         <v>8.08</v>
       </c>
       <c r="J12">
-        <v>8.08</v>
+        <v>1</v>
       </c>
       <c r="K12">
-        <v>8.08</v>
+        <v>8</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M12">
         <v>8</v>
@@ -1333,36 +1215,30 @@
         <v>8</v>
       </c>
       <c r="O12">
-        <v>8</v>
+        <v>8.08</v>
       </c>
       <c r="P12">
-        <v>8</v>
+        <v>8.08</v>
       </c>
       <c r="Q12">
         <v>8.08</v>
       </c>
       <c r="R12">
-        <v>8.08</v>
-      </c>
-      <c r="S12">
-        <v>8.08</v>
-      </c>
-      <c r="T12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
+      <c r="B13">
+        <v>0</v>
       </c>
       <c r="C13">
         <v>9</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E13">
         <v>9</v>
@@ -1371,22 +1247,22 @@
         <v>9</v>
       </c>
       <c r="G13">
-        <v>9</v>
+        <v>9.09</v>
       </c>
       <c r="H13">
-        <v>9</v>
+        <v>9.09</v>
       </c>
       <c r="I13">
         <v>9.09</v>
       </c>
       <c r="J13">
-        <v>9.09</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>9.09</v>
+        <v>9</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M13">
         <v>9</v>
@@ -1395,36 +1271,30 @@
         <v>9</v>
       </c>
       <c r="O13">
-        <v>9</v>
+        <v>9.09</v>
       </c>
       <c r="P13">
-        <v>9</v>
+        <v>9.09</v>
       </c>
       <c r="Q13">
         <v>9.09</v>
       </c>
       <c r="R13">
-        <v>9.09</v>
-      </c>
-      <c r="S13">
-        <v>9.09</v>
-      </c>
-      <c r="T13">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" t="s">
-        <v>14</v>
+      <c r="B14">
+        <v>1</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E14">
         <v>10</v>
@@ -1433,22 +1303,22 @@
         <v>10</v>
       </c>
       <c r="G14">
-        <v>10</v>
+        <v>10.1</v>
       </c>
       <c r="H14">
-        <v>10</v>
+        <v>10.1</v>
       </c>
       <c r="I14">
         <v>10.1</v>
       </c>
       <c r="J14">
-        <v>10.1</v>
+        <v>1</v>
       </c>
       <c r="K14">
-        <v>10.1</v>
+        <v>10</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="M14">
         <v>10</v>
@@ -1457,21 +1327,15 @@
         <v>10</v>
       </c>
       <c r="O14">
-        <v>10</v>
+        <v>10.1</v>
       </c>
       <c r="P14">
-        <v>10</v>
+        <v>10.1</v>
       </c>
       <c r="Q14">
         <v>10.1</v>
       </c>
       <c r="R14">
-        <v>10.1</v>
-      </c>
-      <c r="S14">
-        <v>10.1</v>
-      </c>
-      <c r="T14">
         <v>10</v>
       </c>
     </row>

</xml_diff>